<commit_message>
update cba waste factors
</commit_message>
<xml_diff>
--- a/ssp_modeling/cost-benefits/cb_config_files/cb_config_params.xlsx
+++ b/ssp_modeling/cost-benefits/cb_config_files/cb_config_params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fabianfuentes/git/ssp_mexico/ssp_modeling/cost-benefits/cb_config_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEEAE13A-3FA6-D249-832A-CD0EF2A0F0FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B22CFD6-8403-6446-8AEC-6FA847864C17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33860" yWindow="-600" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-40960" yWindow="-5400" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tx_table" sheetId="1" r:id="rId1"/>
@@ -31,6 +31,9 @@
     <sheet name="attribute_dim_time_period" sheetId="16" r:id="rId16"/>
     <sheet name="attribute_transformation_code" sheetId="17" r:id="rId17"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">cost_factors!$A$1:$L$160</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -6235,7 +6238,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -6245,6 +6248,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6280,13 +6289,14 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -16417,11 +16427,11 @@
   <dimension ref="A1:L160"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B2" sqref="B2"/>
       <selection pane="topRight" activeCell="B2" sqref="B2"/>
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
-      <selection pane="bottomRight" activeCell="C33" sqref="C33"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17232,13 +17242,13 @@
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="4" t="s">
         <v>467</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="4">
         <f>-86/3</f>
         <v>-28.666666666666668</v>
       </c>
@@ -17271,13 +17281,13 @@
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="4" t="s">
         <v>468</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="4">
         <f>-61/3</f>
         <v>-20.333333333333332</v>
       </c>
@@ -17310,13 +17320,13 @@
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="4" t="s">
         <v>469</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24" s="4">
         <f>-70/3</f>
         <v>-23.333333333333332</v>
       </c>
@@ -17349,13 +17359,13 @@
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="4" t="s">
         <v>470</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C25" s="4">
         <f>-57/3</f>
         <v>-19</v>
       </c>
@@ -17388,13 +17398,13 @@
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="4" t="s">
         <v>471</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C26" s="4">
         <f>-7/3</f>
         <v>-2.3333333333333335</v>
       </c>
@@ -17427,13 +17437,13 @@
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="4" t="s">
         <v>472</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C27" s="4">
         <f>-72/3</f>
         <v>-24</v>
       </c>
@@ -17466,13 +17476,13 @@
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="4" t="s">
         <v>473</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C28" s="4">
         <f>-3.04/3</f>
         <v>-1.0133333333333334</v>
       </c>
@@ -17505,13 +17515,13 @@
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="4" t="s">
         <v>474</v>
       </c>
-      <c r="C29" s="3">
+      <c r="C29" s="4">
         <f>-3.04/3</f>
         <v>-1.0133333333333334</v>
       </c>
@@ -17544,13 +17554,13 @@
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="4" t="s">
         <v>475</v>
       </c>
-      <c r="C30" s="3">
+      <c r="C30" s="4">
         <f>-0.64/3</f>
         <v>-0.21333333333333335</v>
       </c>
@@ -17583,13 +17593,13 @@
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="4" t="s">
         <v>476</v>
       </c>
-      <c r="C31" s="3">
+      <c r="C31" s="4">
         <f>-1.44/3</f>
         <v>-0.48</v>
       </c>
@@ -17622,13 +17632,13 @@
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="4" t="s">
         <v>477</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C32" s="4">
         <f>-1.44/3</f>
         <v>-0.48</v>
       </c>
@@ -17661,13 +17671,13 @@
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="4" t="s">
         <v>478</v>
       </c>
-      <c r="C33" s="3">
+      <c r="C33" s="4">
         <f>-0.06/3</f>
         <v>-0.02</v>
       </c>
@@ -18574,14 +18584,15 @@
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+      <c r="A57" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="4" t="s">
         <v>502</v>
       </c>
-      <c r="C57">
-        <v>-500</v>
+      <c r="C57" s="4">
+        <f>-500/3</f>
+        <v>-166.66666666666666</v>
       </c>
       <c r="D57" t="s">
         <v>595</v>
@@ -19373,14 +19384,15 @@
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
+      <c r="A78" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B78" s="4" t="s">
         <v>520</v>
       </c>
-      <c r="C78">
-        <v>-170</v>
+      <c r="C78" s="4">
+        <f>-170/3</f>
+        <v>-56.666666666666664</v>
       </c>
       <c r="D78" t="s">
         <v>591</v>
@@ -19411,14 +19423,15 @@
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
+      <c r="A79" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B79" s="4" t="s">
         <v>521</v>
       </c>
-      <c r="C79">
-        <v>-500</v>
+      <c r="C79" s="4">
+        <f>-500/3</f>
+        <v>-166.66666666666666</v>
       </c>
       <c r="D79" t="s">
         <v>599</v>
@@ -19449,14 +19462,15 @@
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
+      <c r="A80" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B80" s="4" t="s">
         <v>522</v>
       </c>
-      <c r="C80">
-        <v>-500</v>
+      <c r="C80" s="4">
+        <f>-500/3</f>
+        <v>-166.66666666666666</v>
       </c>
       <c r="D80" t="s">
         <v>599</v>
@@ -19829,14 +19843,15 @@
       </c>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A90" t="s">
+      <c r="A90" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B90" s="4" t="s">
         <v>467</v>
       </c>
-      <c r="C90">
-        <v>-86</v>
+      <c r="C90" s="4">
+        <f>-86/3</f>
+        <v>-28.666666666666668</v>
       </c>
       <c r="D90" t="s">
         <v>591</v>
@@ -19867,14 +19882,15 @@
       </c>
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
+      <c r="A91" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B91" s="4" t="s">
         <v>468</v>
       </c>
-      <c r="C91">
-        <v>-86</v>
+      <c r="C91" s="4">
+        <f>-86/3</f>
+        <v>-28.666666666666668</v>
       </c>
       <c r="D91" t="s">
         <v>591</v>
@@ -19905,14 +19921,15 @@
       </c>
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
+      <c r="A92" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B92" s="4" t="s">
         <v>469</v>
       </c>
-      <c r="C92">
-        <v>-86</v>
+      <c r="C92" s="4">
+        <f>-86/3</f>
+        <v>-28.666666666666668</v>
       </c>
       <c r="D92" t="s">
         <v>591</v>
@@ -19943,14 +19960,15 @@
       </c>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
+      <c r="A93" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B93" s="4" t="s">
         <v>470</v>
       </c>
-      <c r="C93">
-        <v>-86</v>
+      <c r="C93" s="4">
+        <f>-86/3</f>
+        <v>-28.666666666666668</v>
       </c>
       <c r="D93" t="s">
         <v>591</v>
@@ -19981,14 +19999,15 @@
       </c>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A94" t="s">
+      <c r="A94" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B94" s="4" t="s">
         <v>471</v>
       </c>
-      <c r="C94">
-        <v>-60.2</v>
+      <c r="C94" s="4">
+        <f>-60.2/3</f>
+        <v>-20.066666666666666</v>
       </c>
       <c r="D94" t="s">
         <v>591</v>
@@ -20019,14 +20038,15 @@
       </c>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A95" t="s">
+      <c r="A95" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B95" s="4" t="s">
         <v>472</v>
       </c>
-      <c r="C95">
-        <v>-60.2</v>
+      <c r="C95" s="4">
+        <f>-60.2/3</f>
+        <v>-20.066666666666666</v>
       </c>
       <c r="D95" t="s">
         <v>591</v>
@@ -21425,14 +21445,15 @@
       </c>
     </row>
     <row r="132" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A132" t="s">
+      <c r="A132" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="B132" t="s">
+      <c r="B132" s="4" t="s">
         <v>558</v>
       </c>
-      <c r="C132">
-        <v>-500000</v>
+      <c r="C132" s="4">
+        <f>-500000/3</f>
+        <v>-166666.66666666666</v>
       </c>
       <c r="D132" t="s">
         <v>353</v>
@@ -22527,6 +22548,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:L160" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <hyperlinks>
     <hyperlink ref="J80" r:id="rId1" location=":~:text=Using%20the%20World%20Bank%20numbers,case%20of%20U.S.%20LMOP%20landfills." xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>

</xml_diff>